<commit_message>
update fig3 qp plot
</commit_message>
<xml_diff>
--- a/plot/fig3/qp_data/QP-5d.xlsx
+++ b/plot/fig3/qp_data/QP-5d.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>Sim-QHD</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>DW-QAA</t>
+  </si>
+  <si>
+    <t>Sim-QAA</t>
   </si>
   <si>
     <t>TNC</t>
@@ -400,13 +403,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +434,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -446,22 +452,25 @@
         <v>0.253</v>
       </c>
       <c r="E2">
+        <v>0.222</v>
+      </c>
+      <c r="F2">
         <v>0.212</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.199</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.185</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.775</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.27</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -475,22 +484,25 @@
         <v>0.266</v>
       </c>
       <c r="E3">
+        <v>0.249</v>
+      </c>
+      <c r="F3">
         <v>0.195</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.194</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.183</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.645</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.268</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -504,22 +516,25 @@
         <v>0.257</v>
       </c>
       <c r="E4">
+        <v>0.267</v>
+      </c>
+      <c r="F4">
         <v>0.274</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.268</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.266</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.52</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.32</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -533,22 +548,25 @@
         <v>0.668</v>
       </c>
       <c r="E5">
+        <v>0.535</v>
+      </c>
+      <c r="F5">
         <v>0.55</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.53</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.498</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.829</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.635</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -562,22 +580,25 @@
         <v>0.461</v>
       </c>
       <c r="E6">
+        <v>0.346</v>
+      </c>
+      <c r="F6">
         <v>0.342</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.333</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.312</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.714</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.395</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -591,22 +612,25 @@
         <v>0.342</v>
       </c>
       <c r="E7">
+        <v>0.32</v>
+      </c>
+      <c r="F7">
         <v>0.303</v>
-      </c>
-      <c r="F7">
-        <v>0.286</v>
       </c>
       <c r="G7">
         <v>0.286</v>
       </c>
       <c r="H7">
+        <v>0.286</v>
+      </c>
+      <c r="I7">
         <v>0.6919999999999999</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.32</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -620,22 +644,25 @@
         <v>0.351</v>
       </c>
       <c r="E8">
+        <v>0.313</v>
+      </c>
+      <c r="F8">
         <v>0.332</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.327</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.318</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.602</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.357</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -649,22 +676,25 @@
         <v>0.428</v>
       </c>
       <c r="E9">
+        <v>0.342</v>
+      </c>
+      <c r="F9">
         <v>0.363</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.349</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.335</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.8100000000000001</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.407</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -678,22 +708,25 @@
         <v>0.508</v>
       </c>
       <c r="E10">
+        <v>0.413</v>
+      </c>
+      <c r="F10">
         <v>0.425</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.418</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.376</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.644</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.508</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -707,18 +740,21 @@
         <v>0.339</v>
       </c>
       <c r="E11">
+        <v>0.288</v>
+      </c>
+      <c r="F11">
         <v>0.273</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.265</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.244</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.654</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.333</v>
       </c>
     </row>
@@ -729,13 +765,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,8 +796,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -775,22 +814,25 @@
         <v>0.0003231935501098633</v>
       </c>
       <c r="E2">
+        <v>0.0003369736671447754</v>
+      </c>
+      <c r="F2">
         <v>0.0004177579879760742</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.0007927116999999999</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.0027022064</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.04792255282402039</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.02720500000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -804,22 +846,25 @@
         <v>0.0003147468566894531</v>
       </c>
       <c r="E3">
+        <v>0.0002719881534576416</v>
+      </c>
+      <c r="F3">
         <v>0.000412569522857666</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.0007282866000000002</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.002481556999999999</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.03248660778999329</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.027878</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -833,22 +878,25 @@
         <v>0.000330233097076416</v>
       </c>
       <c r="E4">
+        <v>0.0003369717597961426</v>
+      </c>
+      <c r="F4">
         <v>0.0003812344074249267</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.0006979268</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.0023460263</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.03079346036911011</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.027469</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -862,22 +910,25 @@
         <v>0.0002771804332733154</v>
       </c>
       <c r="E5">
+        <v>0.0003339846134185791</v>
+      </c>
+      <c r="F5">
         <v>0.0004277808666229248</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.0006864758000000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.002364248700000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.03186353015899658</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.02585900000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -891,22 +942,25 @@
         <v>0.0002932498455047608</v>
       </c>
       <c r="E6">
+        <v>0.0003610746860504151</v>
+      </c>
+      <c r="F6">
         <v>0.0004252591133117676</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.0006735779999999998</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.0023259185</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.03260059928894043</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.02721500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -920,22 +974,25 @@
         <v>0.0003232223987579346</v>
       </c>
       <c r="E7">
+        <v>0.0003179309368133545</v>
+      </c>
+      <c r="F7">
         <v>0.0004012396335601807</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.0006866926999999998</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.0022741283</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.01720727682113648</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.02708600000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -949,22 +1006,25 @@
         <v>0.0003321332931518555</v>
       </c>
       <c r="E8">
+        <v>0.0003499839305877686</v>
+      </c>
+      <c r="F8">
         <v>0.0003950703144073487</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.0006821963000000003</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.0022563321</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.03283646106719971</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.02722800000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -978,22 +1038,25 @@
         <v>0.0003142178058624267</v>
       </c>
       <c r="E9">
+        <v>0.0003230266571044922</v>
+      </c>
+      <c r="F9">
         <v>0.0003862483501434326</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.0006758278999999999</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.002269306600000001</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.03220542311668396</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.02749100000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1007,22 +1070,25 @@
         <v>0.0003272221088409424</v>
       </c>
       <c r="E10">
+        <v>0.0003719723224639892</v>
+      </c>
+      <c r="F10">
         <v>0.000399240255355835</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.0006648017000000002</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.0023262844</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.03254580497741699</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.02853400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1036,18 +1102,21 @@
         <v>0.0003102428913116455</v>
       </c>
       <c r="E11">
+        <v>0.0003407449722290039</v>
+      </c>
+      <c r="F11">
         <v>0.0004247739315032959</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.0006602236999999998</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.002242862599999999</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.022302894115448</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.02626200000000001</v>
       </c>
     </row>
@@ -1058,13 +1127,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,8 +1158,11 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1104,22 +1176,25 @@
         <v>0.005171096801757812</v>
       </c>
       <c r="E2">
+        <v>0.006402499675750732</v>
+      </c>
+      <c r="F2">
         <v>0.008355159759521485</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.0166469457</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.06215074719999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.1916902112960815</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.4080750000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1133,22 +1208,25 @@
         <v>0.004721202850341797</v>
       </c>
       <c r="E3">
+        <v>0.004623798608779907</v>
+      </c>
+      <c r="F3">
         <v>0.009076529502868653</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.0160223052</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.05707581099999998</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.1624330389499664</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.41817</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1162,22 +1240,25 @@
         <v>0.005283729553222656</v>
       </c>
       <c r="E4">
+        <v>0.005054576396942139</v>
+      </c>
+      <c r="F4">
         <v>0.005718516111373901</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.010468902</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.0351903945</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.2155542225837708</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.329628</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1191,22 +1272,25 @@
         <v>0.001385902166366577</v>
       </c>
       <c r="E5">
+        <v>0.002337892293930054</v>
+      </c>
+      <c r="F5">
         <v>0.002566685199737549</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.004805330600000001</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.01654974090000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.09559059047698974</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.129295</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1220,22 +1304,25 @@
         <v>0.002345998764038086</v>
       </c>
       <c r="E6">
+        <v>0.003971821546554566</v>
+      </c>
+      <c r="F6">
         <v>0.005103109359741211</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.008082935999999997</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.0302369405</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.1304023971557617</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.2721500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1249,27 +1336,30 @@
         <v>0.003878668785095215</v>
       </c>
       <c r="E7">
+        <v>0.003815171241760254</v>
+      </c>
+      <c r="F7">
         <v>0.005216115236282349</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.009613697799999998</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.0318377962</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.0688291072845459</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.3250320000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0.00394619607925415</v>
@@ -1278,22 +1368,25 @@
         <v>0.00365346622467041</v>
       </c>
       <c r="E8">
+        <v>0.004549791097640992</v>
+      </c>
+      <c r="F8">
         <v>0.004740843772888184</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.008186355600000004</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.0293323173</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.1641823053359985</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.2995080000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1307,22 +1400,25 @@
         <v>0.002827960252761841</v>
       </c>
       <c r="E9">
+        <v>0.003876319885253906</v>
+      </c>
+      <c r="F9">
         <v>0.004248731851577758</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.007434106899999999</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.02723167920000001</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.09661626935005189</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.2474190000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1336,22 +1432,25 @@
         <v>0.002290554761886597</v>
       </c>
       <c r="E10">
+        <v>0.003347750902175903</v>
+      </c>
+      <c r="F10">
         <v>0.003593162298202515</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.005983215300000001</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.023262844</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.162729024887085</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.1997380000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1365,18 +1464,21 @@
         <v>0.003722914695739746</v>
       </c>
       <c r="E11">
+        <v>0.004770429611206055</v>
+      </c>
+      <c r="F11">
         <v>0.006371608972549439</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.009903355499999997</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.03812866419999999</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.11151447057724</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.3151440000000001</v>
       </c>
     </row>

</xml_diff>